<commit_message>
feat: incluído tabelas de recursos, riscos e responsáveis no excel de portfólio
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/template_portfolio_report_export.xlsx
+++ b/src/main/resources/templates/template_portfolio_report_export.xlsx
@@ -8,17 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmns\Documents\Estudos\Faculdade\TCC\Código\authentication\portplace\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9370513-66B6-4900-9FD1-12E9616174E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC813F66-7327-4ADD-A888-98CDD14AC045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F33266DB-5DB2-474F-8088-4B791CAAF5B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{F33266DB-5DB2-474F-8088-4B791CAAF5B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Projetos" sheetId="1" r:id="rId1"/>
+    <sheet name="Responsáveis" sheetId="2" r:id="rId2"/>
+    <sheet name="Categorias" sheetId="3" r:id="rId3"/>
+    <sheet name="Riscos" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -31,7 +45,7 @@
     <author>ADMIN</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{4B7FE2F3-648B-4FD4-A4C3-0945D98C1142}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{4B7FE2F3-648B-4FD4-A4C3-0945D98C1142}">
       <text>
         <r>
           <rPr>
@@ -51,11 +65,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="I10")</t>
+jx:area(lastCell="I8")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="1" shapeId="0" xr:uid="{CBF03667-FC1E-4976-A444-CFC98C271388}">
+    <comment ref="A13" authorId="1" shapeId="0" xr:uid="{CBF03667-FC1E-4976-A444-CFC98C271388}">
       <text>
         <r>
           <rPr>
@@ -75,11 +89,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell ="N13")</t>
+jx:area(lastCell ="N15")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="1" shapeId="0" xr:uid="{F969A5F1-B44F-44F0-82F0-4C0D05B6822E}">
+    <comment ref="A15" authorId="1" shapeId="0" xr:uid="{F969A5F1-B44F-44F0-82F0-4C0D05B6822E}">
       <text>
         <r>
           <rPr>
@@ -99,7 +113,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="projects" var ="project" lastCell="N13" varIndex="index")</t>
+jx:each(items="projects" var ="project" lastCell="N15" varIndex="index")</t>
         </r>
       </text>
     </comment>
@@ -107,30 +121,257 @@
 </comments>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </valueMetadata>
-</metadata>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gabriel</author>
+    <author>ADMIN</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{A965960A-DA6F-418E-B21E-2967FB3CCC95}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="C5")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="1" shapeId="0" xr:uid="{E1CA42C4-2236-4C85-8161-E3B4D972AC3B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>TRUONGTN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell ="E11")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="1" shapeId="0" xr:uid="{F93CB1E7-E9B7-4D0F-B55D-D06EFD2F5F91}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>TRUONGTN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="portfolio.owners" var ="owner" lastCell="E11" varIndex="index")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gabriel</author>
+    <author>ADMIN</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{2E337ADE-A86D-4860-B4FE-1776D2AB719B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="C5")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="1" shapeId="0" xr:uid="{6D1D1767-6386-4D9C-95B6-D707ABCAF7CB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>TRUONGTN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell ="E11")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="1" shapeId="0" xr:uid="{7863B85E-5B8E-4645-9FDC-505EC1B7EAF0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>TRUONGTN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="portfolio.categories" var ="category" lastCell="E11" varIndex="index")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gabriel</author>
+    <author>ADMIN</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{F0541330-9920-409F-BECB-6D868AFFF868}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="C5")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="1" shapeId="0" xr:uid="{73DC45B8-3626-4917-8864-6A714AA5AD52}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>TRUONGTN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell ="K11")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="1" shapeId="0" xr:uid="{2C4A3427-311F-4006-937E-8F7E48C83294}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>TRUONGTN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="portfolio.risks" var ="risk" lastCell="K11" varIndex="index")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
   <si>
     <t>PROJETOS</t>
   </si>
@@ -241,6 +482,126 @@
   </si>
   <si>
     <t>${portfolio.budget}</t>
+  </si>
+  <si>
+    <t>Qtde. De Projetos</t>
+  </si>
+  <si>
+    <t>Qtde. Responsáveis</t>
+  </si>
+  <si>
+    <t>RESPONSÁVEIS</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>${owner.id}</t>
+  </si>
+  <si>
+    <t>${owner.name}</t>
+  </si>
+  <si>
+    <t>${owner.email}</t>
+  </si>
+  <si>
+    <t>${owner.status}</t>
+  </si>
+  <si>
+    <t>${owner.role}</t>
+  </si>
+  <si>
+    <t>Qtde.  de Categorias</t>
+  </si>
+  <si>
+    <t>CATEGORIAS</t>
+  </si>
+  <si>
+    <t>PODE SER DELETADA?</t>
+  </si>
+  <si>
+    <t>DELETADA?</t>
+  </si>
+  <si>
+    <t>${category.id}</t>
+  </si>
+  <si>
+    <t>${category.name}</t>
+  </si>
+  <si>
+    <t>${category.canBeDeleted}</t>
+  </si>
+  <si>
+    <t>${category.disabled}</t>
+  </si>
+  <si>
+    <t>RISCOS</t>
+  </si>
+  <si>
+    <t>${risk.id}</t>
+  </si>
+  <si>
+    <t>PROBABILIDADE</t>
+  </si>
+  <si>
+    <t>IMPACTO</t>
+  </si>
+  <si>
+    <t>DESCRIÇÃO PROBABILIDADE</t>
+  </si>
+  <si>
+    <t>DESCRIÇÃO IMPACTO</t>
+  </si>
+  <si>
+    <t>SEVERIDADE</t>
+  </si>
+  <si>
+    <t>PLANO DE PREVENÇÃO</t>
+  </si>
+  <si>
+    <t>PLANO DE CONTINGÊNCIA</t>
+  </si>
+  <si>
+    <t>QTDE. DE OCORRÊNCIAS</t>
+  </si>
+  <si>
+    <t>${risk.name}</t>
+  </si>
+  <si>
+    <t>${risk.description}</t>
+  </si>
+  <si>
+    <t>${risk.probabilityDescription}</t>
+  </si>
+  <si>
+    <t>${risk.impactDescription}</t>
+  </si>
+  <si>
+    <t>${risk.preventionPlan}</t>
+  </si>
+  <si>
+    <t>${risk.contingencyPlan}</t>
+  </si>
+  <si>
+    <t>${risk.occurrences.size()}</t>
+  </si>
+  <si>
+    <t>Qtde.  de Riscos</t>
+  </si>
+  <si>
+    <t>${risk.probability.getValue()}</t>
+  </si>
+  <si>
+    <t>${risk.impact.getValue()}</t>
+  </si>
+  <si>
+    <t>${risk.severity}</t>
+  </si>
+  <si>
+    <t>${category.description}</t>
   </si>
 </sst>
 </file>
@@ -250,7 +611,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,6 +682,12 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -542,7 +909,7 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -556,6 +923,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,11 +956,13 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -595,7 +970,158 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título" xfId="2" builtinId="15"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="70">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="9"/>
@@ -628,6 +1154,841 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="7"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="7"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="7"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="7"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="7"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="7"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="7"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF8EA9DB"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF8EA9DB"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF8EA9DB"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1101,88 +2462,72 @@
 </styleSheet>
 </file>
 
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C34785BF-5C18-4F0F-B544-F8A1D97DD983}" name="Projetos" displayName="Projetos" ref="A14:N15" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68" tableBorderDxfId="67">
+  <autoFilter ref="A14:N15" xr:uid="{C34785BF-5C18-4F0F-B544-F8A1D97DD983}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{B9982F39-C6A8-4284-8908-4E644C65F922}" name="ID" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{5C18DBE4-C3FA-4FAB-A309-BAAA96A1D69F}" name="NOME" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{D57071D4-F79A-4BE3-808D-58983FE29527}" name="DESCRIÇÃO" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{3330C946-6589-4A46-8534-08EFBB995296}" name="STATUS" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{F549B89E-15CB-4579-A364-87EFCF07C80F}" name="PAYBACK" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{A848C008-413D-4C4D-B58A-6E60F392C65A}" name="ROI" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{1CFF7D57-C8D2-42C1-86F0-1115A44DF8ED}" name="INICIO" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{F52783B0-0FB0-46DD-B61D-BA0D6E62DB41}" name="FIM" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{44FDBC08-7C76-4210-9B6A-024968068CC1}" name="PV" dataDxfId="58"/>
+    <tableColumn id="10" xr3:uid="{E16EB94D-B2E0-49C5-B0D6-867A4FF9A56F}" name="EV" dataDxfId="57"/>
+    <tableColumn id="11" xr3:uid="{A4CD22A3-69AE-4D1B-9974-710F9195E91D}" name="AC" dataDxfId="56"/>
+    <tableColumn id="12" xr3:uid="{68D3146B-2CFE-4BA0-A50D-40AA837B417B}" name="BAC" dataDxfId="55"/>
+    <tableColumn id="13" xr3:uid="{49777187-662B-45AE-9B7A-141D0A1AC16E}" name="COMPLETION" dataDxfId="54"/>
+    <tableColumn id="14" xr3:uid="{D95B9882-9B64-49CC-9FF6-04FB06C6A633}" name="CPI" dataDxfId="53"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <v>0</v>
-    <v>5</v>
-  </rv>
-</rvData>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FC9C8EEE-7784-45AF-B1B4-0F24B457F8D3}" name="Responsáveis" displayName="Responsáveis" ref="A10:E11" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51" tableBorderDxfId="50">
+  <autoFilter ref="A10:E11" xr:uid="{C34785BF-5C18-4F0F-B544-F8A1D97DD983}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{E910B1DA-CDED-458E-9505-7FE5D479F915}" name="ID" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{B17284BC-E5CE-4F3A-A64B-9970171325AC}" name="NOME" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{4AB70CA7-745E-49CD-B086-659AF6A68788}" name="EMAIL" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{228F786A-1D13-4096-B854-49173AACB059}" name="STATUS" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{0AD34F3E-B71A-467A-9695-23D2ADD54E1E}" name="TIPO" dataDxfId="45"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
-</rvStructures>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0220F4E6-2818-4001-91C2-885D4511F504}" name="Categorias" displayName="Categorias" ref="A10:E11" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42">
+  <autoFilter ref="A10:E11" xr:uid="{C34785BF-5C18-4F0F-B544-F8A1D97DD983}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{73925EED-DB9C-46C8-A1F0-606ADCF84FD5}" name="ID" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{6BE01363-7793-49E3-AF32-88F40C20C64A}" name="NOME" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{26FA878E-8991-44CC-9065-1B8E8B6AEE03}" name="DESCRIÇÃO" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{B878D7D7-802C-4EC2-8CC6-A3BB026A1D53}" name="PODE SER DELETADA?" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{7D41C6FC-6FBD-4249-9A43-D0232DC3595B}" name="DELETADA?" dataDxfId="37"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
-<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
-<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rel r:id="rId1"/>
-</richValueRels>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C34785BF-5C18-4F0F-B544-F8A1D97DD983}" name="Tabela2" displayName="Tabela2" ref="A12:N13" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
-  <autoFilter ref="A12:N13" xr:uid="{C34785BF-5C18-4F0F-B544-F8A1D97DD983}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{B9982F39-C6A8-4284-8908-4E644C65F922}" name="ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{5C18DBE4-C3FA-4FAB-A309-BAAA96A1D69F}" name="NOME" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{D57071D4-F79A-4BE3-808D-58983FE29527}" name="DESCRIÇÃO" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{3330C946-6589-4A46-8534-08EFBB995296}" name="STATUS" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{F549B89E-15CB-4579-A364-87EFCF07C80F}" name="PAYBACK" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{A848C008-413D-4C4D-B58A-6E60F392C65A}" name="ROI" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{1CFF7D57-C8D2-42C1-86F0-1115A44DF8ED}" name="INICIO" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{F52783B0-0FB0-46DD-B61D-BA0D6E62DB41}" name="FIM" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{44FDBC08-7C76-4210-9B6A-024968068CC1}" name="PV" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{E16EB94D-B2E0-49C5-B0D6-867A4FF9A56F}" name="EV" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{A4CD22A3-69AE-4D1B-9974-710F9195E91D}" name="AC" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{68D3146B-2CFE-4BA0-A50D-40AA837B417B}" name="BAC" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{49777187-662B-45AE-9B7A-141D0A1AC16E}" name="COMPLETION" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{D95B9882-9B64-49CC-9FF6-04FB06C6A633}" name="CPI" dataDxfId="3"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C33B0FCC-7653-48A3-AA27-5172435822A4}" name="Riscos" displayName="Riscos" ref="A10:K11" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" tableBorderDxfId="34">
+  <autoFilter ref="A10:K11" xr:uid="{C34785BF-5C18-4F0F-B544-F8A1D97DD983}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{3CE6F104-0202-415E-8E9E-6BF613E3F5A9}" name="ID" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{CD454527-DC22-45A6-B262-4178D443FE74}" name="NOME" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{6AEDE7F5-49FA-424E-8B15-7CEA4C1E8661}" name="DESCRIÇÃO" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{C84A64A8-3430-4538-9D01-8B8E5A7B921C}" name="PROBABILIDADE" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{999A39FC-6C0F-466C-A12A-5ED1809E296A}" name="IMPACTO" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{B1D48DF8-A304-4FA8-B0D6-8EB352A8E6AE}" name="SEVERIDADE"/>
+    <tableColumn id="6" xr3:uid="{08616A4E-8FF0-44A2-A632-AE0F8C408D96}" name="DESCRIÇÃO PROBABILIDADE" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{70F73F7F-70D8-4959-8054-4ECA2F1302DA}" name="DESCRIÇÃO IMPACTO" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{0C95EEF6-D366-4084-AD18-758D37EABDB2}" name="PLANO DE PREVENÇÃO" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{C144F1A5-039D-4901-B5E9-75F652FAA84D}" name="PLANO DE CONTINGÊNCIA" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{324F02E1-388C-46C1-A8C8-0F1D75DFBD52}" name="QTDE. DE OCORRÊNCIAS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1485,10 +2830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F40540-E94A-4819-8B0F-4F635C573AF0}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,193 +2854,606 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E1" s="18" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="B3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-    </row>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+      <c r="G6" s="12"/>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F7" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
-    </row>
-    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <f>COUNTA(Projetos[ID])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A13" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="17"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="19"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="L14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M12" s="7" t="s">
+      <c r="M14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N12" s="8" t="s">
+      <c r="N14" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="M15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="N15" s="6" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B5:F6"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="A11:N11"/>
-    <mergeCell ref="E1:G3"/>
+  <mergeCells count="4">
+    <mergeCell ref="B3:F4"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="A13:N13"/>
   </mergeCells>
-  <conditionalFormatting sqref="B8 D8">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="B6 D6">
+    <cfRule type="cellIs" dxfId="28" priority="13" operator="equal">
+      <formula>"YELLOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="14" operator="equal">
+      <formula>"GREEN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="15" operator="equal">
       <formula>"RED"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="cellIs" dxfId="25" priority="10" operator="equal">
+      <formula>"YELLOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
       <formula>"GREEN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
+      <formula>"RED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409313D8-6283-41E9-9025-2BF3129CCCD7}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <f>COUNTA(Responsáveis[ID])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:E4"/>
+    <mergeCell ref="A9:E9"/>
+  </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"YELLOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+      <formula>"GREEN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+      <formula>"RED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A658CA3-E938-4BB3-B3D6-8C97CFB399AF}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <f>COUNTA(Categorias[ID])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:E4"/>
+    <mergeCell ref="A9:E9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+      <formula>"YELLOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+      <formula>"GREEN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>"RED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14FF48A-C539-41CA-BFCD-67FA7DE31A73}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="6" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:11" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <f>COUNTA(Riscos[ID])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:E4"/>
+    <mergeCell ref="A9:K9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"YELLOW"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"GREEN"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"RED"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>